<commit_message>
chore: update input file of TDD case2 to last version
Updated input files used to run the test case 2 for the TDD to the last version already available in folder ..\source_code\input_files\input_file_template.

modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_1_coupling.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_1_input.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_1_operation.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_definition.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_diagnostic.xlsx
modified:   ../TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_grid.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_diagnostic.xlsx
+++ b/TDD_examples/CASE_2_ENEA_HTS_CICC/conductor_diagnostic.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia.viarengo\Desktop\SC2_1\Description_of_Components\Cavo_ENEA_input_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_2_ENEA_HTS_CICC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD72BB3E-03DA-463F-A842-C49F1A6DDEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DF64A8-1F57-41AC-9A6F-E1612127B5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Space" sheetId="1" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" r:id="rId2"/>
+    <sheet name="Spatial_distribution" sheetId="1" r:id="rId1"/>
+    <sheet name="Time_evolution" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,56 +232,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -619,73 +602,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="str">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="str">
         <f>[1]CONDUCTOR_files!$A$1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="17">
+      <c r="B1" s="13">
         <f>SUM(E2:E2)</f>
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="11">
+      <c r="E1" s="9">
         <f>[1]CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="11">
+      <c r="E2" s="9">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="str">
         <f>[2]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="10" t="str">
+      <c r="B3" s="8" t="str">
         <f>[2]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="10" t="str">
+      <c r="C3" s="8" t="str">
         <f>[2]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="10" t="str">
+      <c r="D3" s="8" t="str">
         <f>[2]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="11" t="str">
+      <c r="E3" s="9" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -694,14 +677,14 @@
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -712,11 +695,11 @@
         <v>2</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -726,12 +709,12 @@
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="5">
         <f>E5+0.05</f>
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -741,12 +724,12 @@
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="5">
         <f t="shared" ref="E7:E26" si="0">E6+0.05</f>
         <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -756,12 +739,12 @@
       <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>2.1499999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -771,12 +754,12 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>2.1999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -786,12 +769,12 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>2.2499999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -801,12 +784,12 @@
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>2.2999999999999989</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -816,12 +799,12 @@
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>2.3499999999999988</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -831,12 +814,12 @@
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="5">
         <f t="shared" si="0"/>
         <v>2.3999999999999986</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -846,12 +829,12 @@
       <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="5">
         <f t="shared" si="0"/>
         <v>2.4499999999999984</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -861,12 +844,12 @@
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="5">
         <f>E14+0.05</f>
         <v>2.4999999999999982</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -876,12 +859,12 @@
       <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="5">
         <f t="shared" si="0"/>
         <v>2.549999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -891,12 +874,12 @@
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="5">
         <f t="shared" si="0"/>
         <v>2.5999999999999979</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
@@ -906,12 +889,12 @@
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>2.6499999999999977</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>33</v>
       </c>
@@ -921,12 +904,12 @@
       <c r="C19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="5">
         <f>E18+0.05</f>
         <v>2.6999999999999975</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -936,12 +919,12 @@
       <c r="C20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="5">
         <f t="shared" si="0"/>
         <v>2.7499999999999973</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
@@ -951,12 +934,12 @@
       <c r="C21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="5">
         <f t="shared" si="0"/>
         <v>2.7999999999999972</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -966,12 +949,12 @@
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="5">
         <f>E21+0.05</f>
         <v>2.849999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -981,12 +964,12 @@
       <c r="C23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="5">
         <f t="shared" si="0"/>
         <v>2.8999999999999968</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -996,12 +979,12 @@
       <c r="C24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="5">
         <f>E23+0.05</f>
         <v>2.9499999999999966</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
@@ -1011,12 +994,12 @@
       <c r="C25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="5">
         <f t="shared" si="0"/>
         <v>2.9999999999999964</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1009,7 @@
       <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="5">
         <f t="shared" si="0"/>
         <v>3.0499999999999963</v>
       </c>
@@ -1043,276 +1026,276 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E6858-601C-4654-9D3B-60211F710697}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="E14" sqref="E14:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="8.88671875" style="13"/>
-    <col min="13" max="16384" width="8.88671875" style="4"/>
+    <col min="6" max="12" width="8.85546875" style="5"/>
+    <col min="13" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="str">
-        <f>Space!A1</f>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="str">
+        <f>Spatial_distribution!A1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="11">
-        <f>Space!B1</f>
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11">
-        <f>Space!E1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11">
-        <f>Space!E2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="str">
-        <f>Space!A3</f>
+      <c r="B1" s="9">
+        <f>Spatial_distribution!B1</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="9">
+        <f>Spatial_distribution!E1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9">
+        <f>Spatial_distribution!E2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="str">
+        <f>Spatial_distribution!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="9" t="str">
-        <f>Space!B3</f>
+      <c r="B3" s="7" t="str">
+        <f>Spatial_distribution!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="9" t="str">
-        <f>Space!C3</f>
+      <c r="C3" s="7" t="str">
+        <f>Spatial_distribution!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="9" t="str">
-        <f>Space!D3</f>
+      <c r="D3" s="7" t="str">
+        <f>Spatial_distribution!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="11" t="str">
-        <f>Space!E3</f>
+      <c r="E3" s="9" t="str">
+        <f>Spatial_distribution!E3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="18">
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12">
         <f>E4+0.3</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12">
         <f t="shared" ref="E6:E7" si="0">E5+0.3</f>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="12">
         <v>1.4750000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12">
         <f>E8+0.01</f>
         <v>1.4850000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="C10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12">
         <f t="shared" ref="E10:E12" si="1">E9+0.01</f>
         <v>1.4950000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12">
         <f t="shared" si="1"/>
         <v>1.5050000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="12">
         <f t="shared" si="1"/>
         <v>1.5150000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="18">
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12">
         <f>E12+0.01</f>
         <v>1.5250000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="18">
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="12">
         <f>1.8</f>
         <v>1.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="18">
+      <c r="C15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12">
         <f>E14+0.3</f>
         <v>2.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="18">
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="12">
         <f t="shared" ref="E16:E17" si="2">E15+0.3</f>
         <v>2.4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12">
         <f t="shared" si="2"/>
         <v>2.6999999999999997</v>
       </c>

</xml_diff>